<commit_message>
database requests (doesn't work)
database requests but they aren't working YET
</commit_message>
<xml_diff>
--- a/Munkafüzet1.xlsx
+++ b/Munkafüzet1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gamen\Desktop\info\Programozás\TSP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gamen\Desktop\info\trading-simulator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3F66BCBE-D393-4739-9664-B30D64A76CE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F672DC7-A222-4484-8401-75224DE7D6B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{7F5CA713-E007-47E0-B8DB-57146DF3953F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
   <si>
     <t>ID</t>
   </si>
@@ -85,6 +85,33 @@
   </si>
   <si>
     <t>current price</t>
+  </si>
+  <si>
+    <t>username</t>
+  </si>
+  <si>
+    <t>passw</t>
+  </si>
+  <si>
+    <t>currency</t>
+  </si>
+  <si>
+    <t>currencyValue</t>
+  </si>
+  <si>
+    <t>pair</t>
+  </si>
+  <si>
+    <t>pairValue</t>
+  </si>
+  <si>
+    <t>tokenValue</t>
+  </si>
+  <si>
+    <t>str</t>
+  </si>
+  <si>
+    <t>float</t>
   </si>
 </sst>
 </file>
@@ -463,15 +490,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E8AF0F7-DC2E-4FC6-A858-92ED933B6420}">
-  <dimension ref="A1:O4"/>
+  <dimension ref="A1:O10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:O4"/>
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="2" max="2" width="15.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6328125" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="13" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14.36328125" customWidth="1"/>
     <col min="15" max="15" width="11.453125" bestFit="1" customWidth="1"/>
@@ -607,6 +636,55 @@
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
     </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{6145C557-C52E-4F97-B0F0-5884749BECE8}"/>

</xml_diff>